<commit_message>
end n fold validation
</commit_message>
<xml_diff>
--- a/data/sumup/results.xlsx
+++ b/data/sumup/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="16065" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="klasyczne podejscie " sheetId="1" r:id="rId1"/>
@@ -17,6 +17,17 @@
     <sheet name="n fold 250 500" sheetId="4" r:id="rId3"/>
     <sheet name="n fold chart" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'klasyczne podejscie '!$F$6:$F$16</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'klasyczne podejscie '!$K$55</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'klasyczne podejscie '!$K$56:$K$66</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'klasyczne podejscie '!$L$55</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'klasyczne podejscie '!$L$56:$L$66</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'klasyczne podejscie '!$M$55</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'klasyczne podejscie '!$M$56:$M$66</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'klasyczne podejscie '!$N$55</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'klasyczne podejscie '!$N$56:$N$66</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -430,25 +441,25 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dane wyjściowe" xfId="3" builtinId="21"/>
@@ -1164,6 +1175,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Crossvalidation step 250 size 500</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1197,8 +1238,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1215,17 +1257,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'n fold chart'!$B$15:$B$21</c:f>
@@ -1285,7 +1325,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-96F3-400F-9A49-3E30A33C7C96}"/>
@@ -1307,17 +1346,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'n fold chart'!$B$15:$B$21</c:f>
@@ -1377,7 +1414,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-96F3-400F-9A49-3E30A33C7C96}"/>
@@ -1399,17 +1435,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'n fold chart'!$B$15:$B$21</c:f>
@@ -1469,7 +1503,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-96F3-400F-9A49-3E30A33C7C96}"/>
@@ -1491,17 +1524,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'n fold chart'!$B$15:$B$21</c:f>
@@ -1561,7 +1592,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-96F3-400F-9A49-3E30A33C7C96}"/>
@@ -1583,17 +1613,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'n fold chart'!$B$15:$B$21</c:f>
@@ -1653,7 +1681,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-96F3-400F-9A49-3E30A33C7C96}"/>
@@ -1675,17 +1702,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'n fold chart'!$B$15:$B$21</c:f>
@@ -1745,7 +1770,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-96F3-400F-9A49-3E30A33C7C96}"/>
@@ -1760,10 +1784,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="1966265343"/>
         <c:axId val="1966263679"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="1966265343"/>
         <c:scaling>
@@ -5931,9 +5955,20 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.4565405169425558E-2"/>
+          <c:y val="0.13475022706630338"/>
+          <c:w val="0.8454082099953748"/>
+          <c:h val="0.44997432541640742"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="4"/>
@@ -5949,9 +5984,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'klasyczne podejscie '!$F$6:$F$16</c:f>
@@ -6035,7 +6068,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-073B-44FA-80B5-5A0814C5828F}"/>
@@ -6056,9 +6088,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'klasyczne podejscie '!$L$56:$L$66</c:f>
@@ -6101,7 +6131,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-073B-44FA-80B5-5A0814C5828F}"/>
@@ -6122,9 +6151,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'klasyczne podejscie '!$M$56:$M$66</c:f>
@@ -6167,7 +6194,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-073B-44FA-80B5-5A0814C5828F}"/>
@@ -6188,9 +6214,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'klasyczne podejscie '!$N$56:$N$66</c:f>
@@ -6233,7 +6257,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-073B-44FA-80B5-5A0814C5828F}"/>
@@ -6248,10 +6271,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="2027328287"/>
         <c:axId val="2027324959"/>
-      </c:lineChart>
+      </c:barChart>
       <c:catAx>
         <c:axId val="2027328287"/>
         <c:scaling>
@@ -6260,6 +6283,31 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>model</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -6269,26 +6317,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -6357,6 +6385,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>accuracy </a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -6366,26 +6419,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -10119,8 +10152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AP102" sqref="AP102"/>
+    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="AH85" sqref="AH85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10145,21 +10178,21 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="14">
         <v>8</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6">
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14">
         <v>16</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -10168,39 +10201,39 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>512</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>256</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>128</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>64</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>512</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>256</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>128</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="1">
@@ -10229,8 +10262,8 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="1">
@@ -10259,8 +10292,8 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G8" s="1">
@@ -10289,8 +10322,8 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E9" s="2"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G9" s="1">
@@ -10319,8 +10352,8 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E10" s="2"/>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G10" s="1">
@@ -10349,8 +10382,8 @@
       </c>
     </row>
     <row r="11" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="1">
@@ -10379,8 +10412,8 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-      <c r="F12" s="4" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="1">
@@ -10409,10 +10442,10 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="1">
@@ -10441,8 +10474,8 @@
       </c>
     </row>
     <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E14" s="2"/>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="1">
@@ -10471,8 +10504,8 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E15" s="2"/>
-      <c r="F15" s="4" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="1">
@@ -10501,8 +10534,8 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E16" s="2"/>
-      <c r="F16" s="4" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="1">
@@ -10531,7 +10564,7 @@
       </c>
     </row>
     <row r="17" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F17" s="4"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -10542,76 +10575,76 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E18" s="3"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
     </row>
     <row r="19" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F20" s="4"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="14">
         <v>8</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6">
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14">
         <v>16</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
     </row>
     <row r="22" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>512</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="4">
         <v>256</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="4">
         <v>128</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="4">
         <v>64</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="4">
         <v>512</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L22" s="4">
         <v>256</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="4">
         <v>128</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="4">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="1">
@@ -10640,8 +10673,8 @@
       </c>
     </row>
     <row r="24" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E24" s="2"/>
-      <c r="F24" s="4" t="s">
+      <c r="E24" s="12"/>
+      <c r="F24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G24" s="1">
@@ -10670,8 +10703,8 @@
       </c>
     </row>
     <row r="25" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E25" s="2"/>
-      <c r="F25" s="4" t="s">
+      <c r="E25" s="12"/>
+      <c r="F25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="1">
@@ -10700,8 +10733,8 @@
       </c>
     </row>
     <row r="26" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E26" s="2"/>
-      <c r="F26" s="4" t="s">
+      <c r="E26" s="12"/>
+      <c r="F26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G26" s="1">
@@ -10730,8 +10763,8 @@
       </c>
     </row>
     <row r="27" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E27" s="2"/>
-      <c r="F27" s="4" t="s">
+      <c r="E27" s="12"/>
+      <c r="F27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G27" s="1">
@@ -10760,8 +10793,8 @@
       </c>
     </row>
     <row r="28" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E28" s="2"/>
-      <c r="F28" s="4" t="s">
+      <c r="E28" s="12"/>
+      <c r="F28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G28" s="1">
@@ -10790,8 +10823,8 @@
       </c>
     </row>
     <row r="29" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E29" s="2"/>
-      <c r="F29" s="4" t="s">
+      <c r="E29" s="12"/>
+      <c r="F29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G29" s="1">
@@ -10820,10 +10853,10 @@
       </c>
     </row>
     <row r="30" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G30" s="1">
@@ -10852,8 +10885,8 @@
       </c>
     </row>
     <row r="31" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E31" s="2"/>
-      <c r="F31" s="4" t="s">
+      <c r="E31" s="12"/>
+      <c r="F31" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G31" s="1">
@@ -10882,8 +10915,8 @@
       </c>
     </row>
     <row r="32" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E32" s="2"/>
-      <c r="F32" s="4" t="s">
+      <c r="E32" s="12"/>
+      <c r="F32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G32" s="1">
@@ -10912,8 +10945,8 @@
       </c>
     </row>
     <row r="33" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E33" s="2"/>
-      <c r="F33" s="4" t="s">
+      <c r="E33" s="12"/>
+      <c r="F33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="1">
@@ -10942,76 +10975,76 @@
       </c>
     </row>
     <row r="34" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F34" s="4"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E35" s="3"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="37" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="14">
         <v>8</v>
       </c>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6">
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14">
         <v>16</v>
       </c>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
     </row>
     <row r="38" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="4">
         <v>512</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="4">
         <v>256</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I38" s="4">
         <v>128</v>
       </c>
-      <c r="J38" s="5">
+      <c r="J38" s="4">
         <v>64</v>
       </c>
-      <c r="K38" s="5">
+      <c r="K38" s="4">
         <v>512</v>
       </c>
-      <c r="L38" s="5">
+      <c r="L38" s="4">
         <v>256</v>
       </c>
-      <c r="M38" s="5">
+      <c r="M38" s="4">
         <v>128</v>
       </c>
-      <c r="N38" s="5">
+      <c r="N38" s="4">
         <v>64</v>
       </c>
     </row>
     <row r="39" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G39" s="1">
@@ -11040,8 +11073,8 @@
       </c>
     </row>
     <row r="40" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="2"/>
-      <c r="F40" s="4" t="s">
+      <c r="E40" s="12"/>
+      <c r="F40" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G40" s="1">
@@ -11070,8 +11103,8 @@
       </c>
     </row>
     <row r="41" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E41" s="2"/>
-      <c r="F41" s="4" t="s">
+      <c r="E41" s="12"/>
+      <c r="F41" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G41" s="1">
@@ -11100,8 +11133,8 @@
       </c>
     </row>
     <row r="42" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E42" s="2"/>
-      <c r="F42" s="4" t="s">
+      <c r="E42" s="12"/>
+      <c r="F42" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G42" s="1">
@@ -11130,8 +11163,8 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E43" s="2"/>
-      <c r="F43" s="4" t="s">
+      <c r="E43" s="12"/>
+      <c r="F43" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G43" s="1">
@@ -11160,8 +11193,8 @@
       </c>
     </row>
     <row r="44" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E44" s="2"/>
-      <c r="F44" s="4" t="s">
+      <c r="E44" s="12"/>
+      <c r="F44" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G44" s="1">
@@ -11190,8 +11223,8 @@
       </c>
     </row>
     <row r="45" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E45" s="2"/>
-      <c r="F45" s="4" t="s">
+      <c r="E45" s="12"/>
+      <c r="F45" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G45" s="1">
@@ -11220,10 +11253,10 @@
       </c>
     </row>
     <row r="46" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G46" s="1">
@@ -11252,8 +11285,8 @@
       </c>
     </row>
     <row r="47" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E47" s="2"/>
-      <c r="F47" s="4" t="s">
+      <c r="E47" s="12"/>
+      <c r="F47" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G47" s="1">
@@ -11282,8 +11315,8 @@
       </c>
     </row>
     <row r="48" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E48" s="2"/>
-      <c r="F48" s="4" t="s">
+      <c r="E48" s="12"/>
+      <c r="F48" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G48" s="1">
@@ -11312,8 +11345,8 @@
       </c>
     </row>
     <row r="49" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E49" s="2"/>
-      <c r="F49" s="4" t="s">
+      <c r="E49" s="12"/>
+      <c r="F49" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G49" s="1">
@@ -11342,7 +11375,7 @@
       </c>
     </row>
     <row r="50" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F50" s="4"/>
+      <c r="F50" s="3"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -11353,19 +11386,19 @@
       <c r="N50" s="1"/>
     </row>
     <row r="51" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E51" s="3"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
     </row>
     <row r="52" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F52" s="4"/>
+      <c r="F52" s="3"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -11376,7 +11409,7 @@
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G53" s="1"/>
@@ -11389,56 +11422,56 @@
       <c r="N53" s="1"/>
     </row>
     <row r="54" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="13">
         <v>8</v>
       </c>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-      <c r="J54" s="9"/>
-      <c r="K54" s="9">
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13">
         <v>16</v>
       </c>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
-      <c r="N54" s="9"/>
+      <c r="L54" s="13"/>
+      <c r="M54" s="13"/>
+      <c r="N54" s="13"/>
     </row>
     <row r="55" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G55" s="10">
+      <c r="G55" s="7">
         <v>512</v>
       </c>
-      <c r="H55" s="10">
+      <c r="H55" s="7">
         <v>256</v>
       </c>
-      <c r="I55" s="10">
+      <c r="I55" s="7">
         <v>128</v>
       </c>
-      <c r="J55" s="10">
+      <c r="J55" s="7">
         <v>64</v>
       </c>
-      <c r="K55" s="10">
+      <c r="K55" s="7">
         <v>512</v>
       </c>
-      <c r="L55" s="10">
+      <c r="L55" s="7">
         <v>256</v>
       </c>
-      <c r="M55" s="10">
+      <c r="M55" s="7">
         <v>128</v>
       </c>
-      <c r="N55" s="10">
+      <c r="N55" s="7">
         <v>64</v>
       </c>
     </row>
     <row r="56" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G56" s="1">
@@ -11467,8 +11500,8 @@
       </c>
     </row>
     <row r="57" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E57" s="2"/>
-      <c r="F57" s="4" t="s">
+      <c r="E57" s="12"/>
+      <c r="F57" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G57" s="1">
@@ -11497,8 +11530,8 @@
       </c>
     </row>
     <row r="58" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E58" s="2"/>
-      <c r="F58" s="4" t="s">
+      <c r="E58" s="12"/>
+      <c r="F58" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G58" s="1">
@@ -11527,8 +11560,8 @@
       </c>
     </row>
     <row r="59" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E59" s="2"/>
-      <c r="F59" s="4" t="s">
+      <c r="E59" s="12"/>
+      <c r="F59" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G59" s="1">
@@ -11557,8 +11590,8 @@
       </c>
     </row>
     <row r="60" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E60" s="2"/>
-      <c r="F60" s="4" t="s">
+      <c r="E60" s="12"/>
+      <c r="F60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G60" s="1">
@@ -11587,8 +11620,8 @@
       </c>
     </row>
     <row r="61" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E61" s="2"/>
-      <c r="F61" s="4" t="s">
+      <c r="E61" s="12"/>
+      <c r="F61" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G61" s="1">
@@ -11617,8 +11650,8 @@
       </c>
     </row>
     <row r="62" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E62" s="2"/>
-      <c r="F62" s="4" t="s">
+      <c r="E62" s="12"/>
+      <c r="F62" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G62" s="1">
@@ -11647,10 +11680,10 @@
       </c>
     </row>
     <row r="63" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G63" s="1">
@@ -11679,8 +11712,8 @@
       </c>
     </row>
     <row r="64" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E64" s="2"/>
-      <c r="F64" s="4" t="s">
+      <c r="E64" s="12"/>
+      <c r="F64" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G64" s="1">
@@ -11709,8 +11742,8 @@
       </c>
     </row>
     <row r="65" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E65" s="2"/>
-      <c r="F65" s="4" t="s">
+      <c r="E65" s="12"/>
+      <c r="F65" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G65" s="1">
@@ -11739,8 +11772,8 @@
       </c>
     </row>
     <row r="66" spans="5:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E66" s="2"/>
-      <c r="F66" s="4" t="s">
+      <c r="E66" s="12"/>
+      <c r="F66" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G66" s="1">
@@ -11770,22 +11803,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:N37"/>
     <mergeCell ref="E63:E66"/>
     <mergeCell ref="E39:E45"/>
     <mergeCell ref="E46:E49"/>
     <mergeCell ref="G54:J54"/>
     <mergeCell ref="K54:N54"/>
     <mergeCell ref="E56:E62"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="E6:E12"/>
-    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11844,135 +11877,135 @@
       </c>
     </row>
     <row r="5" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="Q5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="R5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="S5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="T5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="U5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="V5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="W5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X5" s="11" t="s">
+      <c r="X5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="Y5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Z5" s="11" t="s">
+      <c r="Z5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA5" s="11" t="s">
+      <c r="AA5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" s="11" t="s">
+      <c r="AB5" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC5" s="11" t="s">
+      <c r="AC5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AD5" s="11" t="s">
+      <c r="AD5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AE5" s="11" t="s">
+      <c r="AE5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AF5" s="11" t="s">
+      <c r="AF5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AG5" s="11" t="s">
+      <c r="AG5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH5" s="11" t="s">
+      <c r="AH5" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI5" s="11" t="s">
+      <c r="AI5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ5" s="11" t="s">
+      <c r="AJ5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AK5" s="11" t="s">
+      <c r="AK5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AL5" s="11" t="s">
+      <c r="AL5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AM5" s="11" t="s">
+      <c r="AM5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN5" s="11" t="s">
+      <c r="AN5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AO5" s="11" t="s">
+      <c r="AO5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AP5" s="11" t="s">
+      <c r="AP5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AQ5" s="11" t="s">
+      <c r="AQ5" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1">
@@ -12095,12 +12128,12 @@
       <c r="AP6" s="1">
         <v>0.40909090909090901</v>
       </c>
-      <c r="AQ6" s="12">
+      <c r="AQ6" s="9">
         <v>0.51742424242424201</v>
       </c>
     </row>
     <row r="7" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1">
@@ -12223,12 +12256,12 @@
       <c r="AP7" s="1">
         <v>0.53030303030303005</v>
       </c>
-      <c r="AQ7" s="12">
+      <c r="AQ7" s="9">
         <v>0.52803030303030296</v>
       </c>
     </row>
     <row r="8" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1">
@@ -12351,12 +12384,12 @@
       <c r="AP8" s="1">
         <v>0.42424242424242398</v>
       </c>
-      <c r="AQ8" s="12">
+      <c r="AQ8" s="9">
         <v>0.52196969696969697</v>
       </c>
     </row>
     <row r="9" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1">
@@ -12479,12 +12512,12 @@
       <c r="AP9" s="1">
         <v>0.60606060606060597</v>
       </c>
-      <c r="AQ9" s="12">
+      <c r="AQ9" s="9">
         <v>0.55378787878787805</v>
       </c>
     </row>
     <row r="10" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1">
@@ -12607,12 +12640,12 @@
       <c r="AP10" s="1">
         <v>0.60606060606060597</v>
       </c>
-      <c r="AQ10" s="12">
+      <c r="AQ10" s="9">
         <v>0.58825757575757498</v>
       </c>
     </row>
     <row r="11" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1">
@@ -12735,12 +12768,12 @@
       <c r="AP11" s="1">
         <v>0.56060606060606</v>
       </c>
-      <c r="AQ11" s="12">
+      <c r="AQ11" s="9">
         <v>0.51780303030302999</v>
       </c>
     </row>
     <row r="12" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1">
@@ -12863,7 +12896,7 @@
       <c r="AP12" s="1">
         <v>0.57575757575757502</v>
       </c>
-      <c r="AQ12" s="12">
+      <c r="AQ12" s="9">
         <v>0.52045454545454495</v>
       </c>
     </row>
@@ -12900,135 +12933,135 @@
       </c>
     </row>
     <row r="18" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N18" s="11" t="s">
+      <c r="N18" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O18" s="11" t="s">
+      <c r="O18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P18" s="11" t="s">
+      <c r="P18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q18" s="11" t="s">
+      <c r="Q18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R18" s="11" t="s">
+      <c r="R18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S18" s="11" t="s">
+      <c r="S18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T18" s="11" t="s">
+      <c r="T18" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="U18" s="11" t="s">
+      <c r="U18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V18" s="11" t="s">
+      <c r="V18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W18" s="11" t="s">
+      <c r="W18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X18" s="11" t="s">
+      <c r="X18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y18" s="11" t="s">
+      <c r="Y18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Z18" s="11" t="s">
+      <c r="Z18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA18" s="11" t="s">
+      <c r="AA18" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AB18" s="11" t="s">
+      <c r="AB18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC18" s="11" t="s">
+      <c r="AC18" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AD18" s="11" t="s">
+      <c r="AD18" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AE18" s="11" t="s">
+      <c r="AE18" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AF18" s="11" t="s">
+      <c r="AF18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AG18" s="11" t="s">
+      <c r="AG18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH18" s="11" t="s">
+      <c r="AH18" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI18" s="11" t="s">
+      <c r="AI18" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ18" s="11" t="s">
+      <c r="AJ18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AK18" s="11" t="s">
+      <c r="AK18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AL18" s="11" t="s">
+      <c r="AL18" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AM18" s="11" t="s">
+      <c r="AM18" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN18" s="11" t="s">
+      <c r="AN18" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AO18" s="11" t="s">
+      <c r="AO18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AP18" s="11" t="s">
+      <c r="AP18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AQ18" s="11" t="s">
+      <c r="AQ18" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="1">
@@ -13151,12 +13184,12 @@
       <c r="AP19" s="1">
         <v>0.31818181818181801</v>
       </c>
-      <c r="AQ19" s="12">
+      <c r="AQ19" s="9">
         <v>0.42159090909090902</v>
       </c>
     </row>
     <row r="20" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="1">
@@ -13279,12 +13312,12 @@
       <c r="AP20" s="1">
         <v>0.24242424242424199</v>
       </c>
-      <c r="AQ20" s="12">
+      <c r="AQ20" s="9">
         <v>0.43409090909090903</v>
       </c>
     </row>
     <row r="21" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="1">
@@ -13407,12 +13440,12 @@
       <c r="AP21" s="1">
         <v>0.31818181818181801</v>
       </c>
-      <c r="AQ21" s="12">
+      <c r="AQ21" s="9">
         <v>0.423863636363636</v>
       </c>
     </row>
     <row r="22" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="1">
@@ -13535,12 +13568,12 @@
       <c r="AP22" s="1">
         <v>0.27272727272727199</v>
       </c>
-      <c r="AQ22" s="12">
+      <c r="AQ22" s="9">
         <v>0.460984848484848</v>
       </c>
     </row>
     <row r="23" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="1">
@@ -13663,12 +13696,12 @@
       <c r="AP23" s="1">
         <v>0.27272727272727199</v>
       </c>
-      <c r="AQ23" s="12">
+      <c r="AQ23" s="9">
         <v>0.46136363636363598</v>
       </c>
     </row>
     <row r="24" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="1">
@@ -13791,12 +13824,12 @@
       <c r="AP24" s="1">
         <v>0.31818181818181801</v>
       </c>
-      <c r="AQ24" s="12">
+      <c r="AQ24" s="9">
         <v>0.444318181818181</v>
       </c>
     </row>
     <row r="25" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1">
@@ -13919,7 +13952,7 @@
       <c r="AP25" s="1">
         <v>0.25757575757575701</v>
       </c>
-      <c r="AQ25" s="12">
+      <c r="AQ25" s="9">
         <v>0.44280303030302998</v>
       </c>
     </row>
@@ -13956,135 +13989,135 @@
       </c>
     </row>
     <row r="31" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="11" t="s">
+      <c r="J31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="11" t="s">
+      <c r="K31" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L31" s="11" t="s">
+      <c r="L31" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M31" s="11" t="s">
+      <c r="M31" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N31" s="11" t="s">
+      <c r="N31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O31" s="11" t="s">
+      <c r="O31" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P31" s="11" t="s">
+      <c r="P31" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q31" s="11" t="s">
+      <c r="Q31" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R31" s="11" t="s">
+      <c r="R31" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S31" s="11" t="s">
+      <c r="S31" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T31" s="11" t="s">
+      <c r="T31" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="U31" s="11" t="s">
+      <c r="U31" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V31" s="11" t="s">
+      <c r="V31" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W31" s="11" t="s">
+      <c r="W31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X31" s="11" t="s">
+      <c r="X31" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y31" s="11" t="s">
+      <c r="Y31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Z31" s="11" t="s">
+      <c r="Z31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA31" s="11" t="s">
+      <c r="AA31" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AB31" s="11" t="s">
+      <c r="AB31" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC31" s="11" t="s">
+      <c r="AC31" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AD31" s="11" t="s">
+      <c r="AD31" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AE31" s="11" t="s">
+      <c r="AE31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AF31" s="11" t="s">
+      <c r="AF31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AG31" s="11" t="s">
+      <c r="AG31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH31" s="11" t="s">
+      <c r="AH31" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI31" s="11" t="s">
+      <c r="AI31" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ31" s="11" t="s">
+      <c r="AJ31" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AK31" s="11" t="s">
+      <c r="AK31" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AL31" s="11" t="s">
+      <c r="AL31" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AM31" s="11" t="s">
+      <c r="AM31" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN31" s="11" t="s">
+      <c r="AN31" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AO31" s="11" t="s">
+      <c r="AO31" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AP31" s="11" t="s">
+      <c r="AP31" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AQ31" s="11" t="s">
+      <c r="AQ31" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="1">
@@ -14207,12 +14240,12 @@
       <c r="AP32" s="1">
         <v>0.48484848484848397</v>
       </c>
-      <c r="AQ32" s="12">
+      <c r="AQ32" s="9">
         <v>0.50227272727272698</v>
       </c>
     </row>
     <row r="33" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="1">
@@ -14335,12 +14368,12 @@
       <c r="AP33" s="1">
         <v>0.34848484848484801</v>
       </c>
-      <c r="AQ33" s="12">
+      <c r="AQ33" s="9">
         <v>0.53219696969696895</v>
       </c>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="1">
@@ -14463,12 +14496,12 @@
       <c r="AP34" s="1">
         <v>0.37878787878787801</v>
       </c>
-      <c r="AQ34" s="12">
+      <c r="AQ34" s="9">
         <v>0.49696969696969601</v>
       </c>
     </row>
     <row r="35" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="1">
@@ -14591,12 +14624,12 @@
       <c r="AP35" s="1">
         <v>0.59090909090909005</v>
       </c>
-      <c r="AQ35" s="12">
+      <c r="AQ35" s="9">
         <v>0.58333333333333304</v>
       </c>
     </row>
     <row r="36" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="1">
@@ -14719,12 +14752,12 @@
       <c r="AP36" s="1">
         <v>0.59090909090909005</v>
       </c>
-      <c r="AQ36" s="12">
+      <c r="AQ36" s="9">
         <v>0.62386363636363595</v>
       </c>
     </row>
     <row r="37" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="1">
@@ -14847,12 +14880,12 @@
       <c r="AP37" s="1">
         <v>0.39393939393939298</v>
       </c>
-      <c r="AQ37" s="12">
+      <c r="AQ37" s="9">
         <v>0.48977272727272703</v>
       </c>
     </row>
     <row r="38" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="1">
@@ -14975,7 +15008,7 @@
       <c r="AP38" s="1">
         <v>0.25757575757575701</v>
       </c>
-      <c r="AQ38" s="12">
+      <c r="AQ38" s="9">
         <v>0.47992424242424198</v>
       </c>
     </row>
@@ -15012,135 +15045,135 @@
       </c>
     </row>
     <row r="44" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="G44" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H44" s="11" t="s">
+      <c r="H44" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I44" s="11" t="s">
+      <c r="I44" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J44" s="11" t="s">
+      <c r="J44" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K44" s="11" t="s">
+      <c r="K44" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L44" s="11" t="s">
+      <c r="L44" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M44" s="11" t="s">
+      <c r="M44" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N44" s="11" t="s">
+      <c r="N44" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O44" s="11" t="s">
+      <c r="O44" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P44" s="11" t="s">
+      <c r="P44" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q44" s="11" t="s">
+      <c r="Q44" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R44" s="11" t="s">
+      <c r="R44" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S44" s="11" t="s">
+      <c r="S44" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T44" s="11" t="s">
+      <c r="T44" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="U44" s="11" t="s">
+      <c r="U44" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V44" s="11" t="s">
+      <c r="V44" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W44" s="11" t="s">
+      <c r="W44" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X44" s="11" t="s">
+      <c r="X44" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y44" s="11" t="s">
+      <c r="Y44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Z44" s="11" t="s">
+      <c r="Z44" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA44" s="11" t="s">
+      <c r="AA44" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AB44" s="11" t="s">
+      <c r="AB44" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC44" s="11" t="s">
+      <c r="AC44" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AD44" s="11" t="s">
+      <c r="AD44" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AE44" s="11" t="s">
+      <c r="AE44" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AF44" s="11" t="s">
+      <c r="AF44" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AG44" s="11" t="s">
+      <c r="AG44" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH44" s="11" t="s">
+      <c r="AH44" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI44" s="11" t="s">
+      <c r="AI44" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ44" s="11" t="s">
+      <c r="AJ44" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AK44" s="11" t="s">
+      <c r="AK44" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AL44" s="11" t="s">
+      <c r="AL44" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AM44" s="11" t="s">
+      <c r="AM44" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN44" s="11" t="s">
+      <c r="AN44" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AO44" s="11" t="s">
+      <c r="AO44" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AP44" s="11" t="s">
+      <c r="AP44" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AQ44" s="11" t="s">
+      <c r="AQ44" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C45" s="1">
@@ -15263,12 +15296,12 @@
       <c r="AP45" s="1">
         <v>0.30303030303030298</v>
       </c>
-      <c r="AQ45" s="12">
+      <c r="AQ45" s="9">
         <v>0.39280303030302999</v>
       </c>
     </row>
     <row r="46" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C46" s="1">
@@ -15391,12 +15424,12 @@
       <c r="AP46" s="1">
         <v>0.42424242424242398</v>
       </c>
-      <c r="AQ46" s="12">
+      <c r="AQ46" s="9">
         <v>0.41477272727272702</v>
       </c>
     </row>
     <row r="47" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C47" s="1">
@@ -15519,12 +15552,12 @@
       <c r="AP47" s="1">
         <v>0.51515151515151503</v>
       </c>
-      <c r="AQ47" s="12">
+      <c r="AQ47" s="9">
         <v>0.40681818181818102</v>
       </c>
     </row>
     <row r="48" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="1">
@@ -15647,12 +15680,12 @@
       <c r="AP48" s="1">
         <v>0.45454545454545398</v>
       </c>
-      <c r="AQ48" s="12">
+      <c r="AQ48" s="9">
         <v>0.47499999999999898</v>
       </c>
     </row>
     <row r="49" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="1">
@@ -15775,12 +15808,12 @@
       <c r="AP49" s="1">
         <v>0.45454545454545398</v>
       </c>
-      <c r="AQ49" s="12">
+      <c r="AQ49" s="9">
         <v>0.47992424242424198</v>
       </c>
     </row>
     <row r="50" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="1">
@@ -15903,12 +15936,12 @@
       <c r="AP50" s="1">
         <v>0.40909090909090901</v>
       </c>
-      <c r="AQ50" s="12">
+      <c r="AQ50" s="9">
         <v>0.43522727272727202</v>
       </c>
     </row>
     <row r="51" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="1">
@@ -16031,7 +16064,7 @@
       <c r="AP51" s="1">
         <v>0.40909090909090901</v>
       </c>
-      <c r="AQ51" s="12">
+      <c r="AQ51" s="9">
         <v>0.423863636363636</v>
       </c>
     </row>
@@ -16068,135 +16101,135 @@
       </c>
     </row>
     <row r="57" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D57" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="E57" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G57" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H57" s="11" t="s">
+      <c r="H57" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I57" s="11" t="s">
+      <c r="I57" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J57" s="11" t="s">
+      <c r="J57" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K57" s="11" t="s">
+      <c r="K57" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L57" s="11" t="s">
+      <c r="L57" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M57" s="11" t="s">
+      <c r="M57" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N57" s="11" t="s">
+      <c r="N57" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O57" s="11" t="s">
+      <c r="O57" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P57" s="11" t="s">
+      <c r="P57" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q57" s="11" t="s">
+      <c r="Q57" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R57" s="11" t="s">
+      <c r="R57" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S57" s="11" t="s">
+      <c r="S57" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T57" s="11" t="s">
+      <c r="T57" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="U57" s="11" t="s">
+      <c r="U57" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V57" s="11" t="s">
+      <c r="V57" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W57" s="11" t="s">
+      <c r="W57" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X57" s="11" t="s">
+      <c r="X57" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y57" s="11" t="s">
+      <c r="Y57" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Z57" s="11" t="s">
+      <c r="Z57" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA57" s="11" t="s">
+      <c r="AA57" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AB57" s="11" t="s">
+      <c r="AB57" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC57" s="11" t="s">
+      <c r="AC57" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AD57" s="11" t="s">
+      <c r="AD57" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AE57" s="11" t="s">
+      <c r="AE57" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AF57" s="11" t="s">
+      <c r="AF57" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AG57" s="11" t="s">
+      <c r="AG57" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH57" s="11" t="s">
+      <c r="AH57" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI57" s="11" t="s">
+      <c r="AI57" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ57" s="11" t="s">
+      <c r="AJ57" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AK57" s="11" t="s">
+      <c r="AK57" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AL57" s="11" t="s">
+      <c r="AL57" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AM57" s="11" t="s">
+      <c r="AM57" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN57" s="11" t="s">
+      <c r="AN57" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AO57" s="11" t="s">
+      <c r="AO57" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AP57" s="11" t="s">
+      <c r="AP57" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AQ57" s="11" t="s">
+      <c r="AQ57" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="58" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="1">
@@ -16319,12 +16352,12 @@
       <c r="AP58" s="1">
         <v>0.40909090909090901</v>
       </c>
-      <c r="AQ58" s="12">
+      <c r="AQ58" s="9">
         <v>0.49204545454545401</v>
       </c>
     </row>
     <row r="59" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C59" s="1">
@@ -16447,12 +16480,12 @@
       <c r="AP59" s="1">
         <v>0.439393939393939</v>
       </c>
-      <c r="AQ59" s="12">
+      <c r="AQ59" s="9">
         <v>0.495075757575757</v>
       </c>
     </row>
     <row r="60" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C60" s="1">
@@ -16575,12 +16608,12 @@
       <c r="AP60" s="1">
         <v>0.39393939393939298</v>
       </c>
-      <c r="AQ60" s="12">
+      <c r="AQ60" s="9">
         <v>0.52386363636363598</v>
       </c>
     </row>
     <row r="61" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C61" s="1">
@@ -16703,12 +16736,12 @@
       <c r="AP61" s="1">
         <v>0.57575757575757502</v>
       </c>
-      <c r="AQ61" s="12">
+      <c r="AQ61" s="9">
         <v>0.57348484848484804</v>
       </c>
     </row>
     <row r="62" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C62" s="1">
@@ -16831,12 +16864,12 @@
       <c r="AP62" s="1">
         <v>0.57575757575757502</v>
       </c>
-      <c r="AQ62" s="12">
+      <c r="AQ62" s="9">
         <v>0.63712121212121198</v>
       </c>
     </row>
     <row r="63" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C63" s="1">
@@ -16959,12 +16992,12 @@
       <c r="AP63" s="1">
         <v>0.39393939393939298</v>
       </c>
-      <c r="AQ63" s="12">
+      <c r="AQ63" s="9">
         <v>0.49545454545454498</v>
       </c>
     </row>
     <row r="64" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C64" s="1">
@@ -17087,7 +17120,7 @@
       <c r="AP64" s="1">
         <v>0.27272727272727199</v>
       </c>
-      <c r="AQ64" s="12">
+      <c r="AQ64" s="9">
         <v>0.483333333333333</v>
       </c>
     </row>
@@ -17124,135 +17157,135 @@
       </c>
     </row>
     <row r="70" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D70" s="11" t="s">
+      <c r="D70" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="E70" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G70" s="11" t="s">
+      <c r="G70" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H70" s="11" t="s">
+      <c r="H70" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I70" s="11" t="s">
+      <c r="I70" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J70" s="11" t="s">
+      <c r="J70" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K70" s="11" t="s">
+      <c r="K70" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L70" s="11" t="s">
+      <c r="L70" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M70" s="11" t="s">
+      <c r="M70" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="N70" s="11" t="s">
+      <c r="N70" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O70" s="11" t="s">
+      <c r="O70" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P70" s="11" t="s">
+      <c r="P70" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q70" s="11" t="s">
+      <c r="Q70" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R70" s="11" t="s">
+      <c r="R70" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S70" s="11" t="s">
+      <c r="S70" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="T70" s="11" t="s">
+      <c r="T70" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="U70" s="11" t="s">
+      <c r="U70" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="V70" s="11" t="s">
+      <c r="V70" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W70" s="11" t="s">
+      <c r="W70" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X70" s="11" t="s">
+      <c r="X70" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Y70" s="11" t="s">
+      <c r="Y70" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Z70" s="11" t="s">
+      <c r="Z70" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AA70" s="11" t="s">
+      <c r="AA70" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AB70" s="11" t="s">
+      <c r="AB70" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC70" s="11" t="s">
+      <c r="AC70" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AD70" s="11" t="s">
+      <c r="AD70" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AE70" s="11" t="s">
+      <c r="AE70" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AF70" s="11" t="s">
+      <c r="AF70" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AG70" s="11" t="s">
+      <c r="AG70" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AH70" s="11" t="s">
+      <c r="AH70" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AI70" s="11" t="s">
+      <c r="AI70" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AJ70" s="11" t="s">
+      <c r="AJ70" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AK70" s="11" t="s">
+      <c r="AK70" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AL70" s="11" t="s">
+      <c r="AL70" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AM70" s="11" t="s">
+      <c r="AM70" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AN70" s="11" t="s">
+      <c r="AN70" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AO70" s="11" t="s">
+      <c r="AO70" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AP70" s="11" t="s">
+      <c r="AP70" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AQ70" s="11" t="s">
+      <c r="AQ70" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="71" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C71" s="1">
@@ -17375,12 +17408,12 @@
       <c r="AP71" s="1">
         <v>0.30303030303030298</v>
       </c>
-      <c r="AQ71" s="12">
+      <c r="AQ71" s="9">
         <v>0.391666666666666</v>
       </c>
     </row>
     <row r="72" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C72" s="1">
@@ -17503,12 +17536,12 @@
       <c r="AP72" s="1">
         <v>0.34848484848484801</v>
       </c>
-      <c r="AQ72" s="12">
+      <c r="AQ72" s="9">
         <v>0.44015151515151502</v>
       </c>
     </row>
     <row r="73" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C73" s="1">
@@ -17631,12 +17664,12 @@
       <c r="AP73" s="1">
         <v>0.51515151515151503</v>
       </c>
-      <c r="AQ73" s="12">
+      <c r="AQ73" s="9">
         <v>0.414015151515151</v>
       </c>
     </row>
     <row r="74" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C74" s="1">
@@ -17759,12 +17792,12 @@
       <c r="AP74" s="1">
         <v>0.45454545454545398</v>
       </c>
-      <c r="AQ74" s="12">
+      <c r="AQ74" s="9">
         <v>0.472727272727272</v>
       </c>
     </row>
     <row r="75" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C75" s="1">
@@ -17887,12 +17920,12 @@
       <c r="AP75" s="1">
         <v>0.42424242424242398</v>
       </c>
-      <c r="AQ75" s="12">
+      <c r="AQ75" s="9">
         <v>0.47613636363636302</v>
       </c>
     </row>
     <row r="76" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C76" s="1">
@@ -18015,12 +18048,12 @@
       <c r="AP76" s="1">
         <v>0.45454545454545398</v>
       </c>
-      <c r="AQ76" s="12">
+      <c r="AQ76" s="9">
         <v>0.44545454545454499</v>
       </c>
     </row>
     <row r="77" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C77" s="1">
@@ -18143,7 +18176,7 @@
       <c r="AP77" s="1">
         <v>0.60606060606060597</v>
       </c>
-      <c r="AQ77" s="12">
+      <c r="AQ77" s="9">
         <v>0.43143939393939301</v>
       </c>
     </row>
@@ -18203,60 +18236,60 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="R6" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1">
@@ -18304,12 +18337,12 @@
       <c r="Q7" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="9">
         <v>0.55434343434343403</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1">
@@ -18357,12 +18390,12 @@
       <c r="Q8" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R8" s="12">
+      <c r="R8" s="9">
         <v>0.53696969696969699</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="1">
@@ -18410,12 +18443,12 @@
       <c r="Q9" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R9" s="12">
+      <c r="R9" s="9">
         <v>0.54101010101010105</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="1">
@@ -18463,12 +18496,12 @@
       <c r="Q10" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R10" s="12">
+      <c r="R10" s="9">
         <v>0.61212121212121196</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1">
@@ -18516,12 +18549,12 @@
       <c r="Q11" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R11" s="12">
+      <c r="R11" s="9">
         <v>0.61777777777777698</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1">
@@ -18569,12 +18602,12 @@
       <c r="Q12" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R12" s="12">
+      <c r="R12" s="9">
         <v>0.56525252525252501</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1">
@@ -18622,7 +18655,7 @@
       <c r="Q13" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R13" s="12">
+      <c r="R13" s="9">
         <v>0.55515151515151495</v>
       </c>
     </row>
@@ -18659,60 +18692,60 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="N19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="11" t="s">
+      <c r="O19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="P19" s="11" t="s">
+      <c r="P19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q19" s="11" t="s">
+      <c r="Q19" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R19" s="11" t="s">
+      <c r="R19" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="1">
@@ -18760,12 +18793,12 @@
       <c r="Q20" s="1">
         <v>0.29090909090909001</v>
       </c>
-      <c r="R20" s="12">
+      <c r="R20" s="9">
         <v>0.414545454545454</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="1">
@@ -18813,12 +18846,12 @@
       <c r="Q21" s="1">
         <v>0.236363636363636</v>
       </c>
-      <c r="R21" s="12">
+      <c r="R21" s="9">
         <v>0.41616161616161601</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="1">
@@ -18866,12 +18899,12 @@
       <c r="Q22" s="1">
         <v>0.27878787878787797</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="9">
         <v>0.43030303030303002</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="1">
@@ -18919,12 +18952,12 @@
       <c r="Q23" s="1">
         <v>0.27878787878787797</v>
       </c>
-      <c r="R23" s="12">
+      <c r="R23" s="9">
         <v>0.44282828282828202</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="1">
@@ -18972,12 +19005,12 @@
       <c r="Q24" s="1">
         <v>0.27878787878787797</v>
       </c>
-      <c r="R24" s="12">
+      <c r="R24" s="9">
         <v>0.46343434343434298</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="1">
@@ -19025,12 +19058,12 @@
       <c r="Q25" s="1">
         <v>0.236363636363636</v>
       </c>
-      <c r="R25" s="12">
+      <c r="R25" s="9">
         <v>0.42303030303030298</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="1">
@@ -19078,7 +19111,7 @@
       <c r="Q26" s="1">
         <v>0.21212121212121199</v>
       </c>
-      <c r="R26" s="12">
+      <c r="R26" s="9">
         <v>0.41696969696969599</v>
       </c>
     </row>
@@ -19115,60 +19148,60 @@
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="J32" s="11" t="s">
+      <c r="J32" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L32" s="11" t="s">
+      <c r="L32" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M32" s="11" t="s">
+      <c r="M32" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N32" s="11" t="s">
+      <c r="N32" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O32" s="11" t="s">
+      <c r="O32" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="P32" s="11" t="s">
+      <c r="P32" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q32" s="11" t="s">
+      <c r="Q32" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R32" s="11" t="s">
+      <c r="R32" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="1">
@@ -19216,12 +19249,12 @@
       <c r="Q33" s="1">
         <v>0.30909090909090903</v>
       </c>
-      <c r="R33" s="12">
+      <c r="R33" s="9">
         <v>0.42707070707070699</v>
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="1">
@@ -19269,12 +19302,12 @@
       <c r="Q34" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R34" s="12">
+      <c r="R34" s="9">
         <v>0.49050505050505</v>
       </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="1">
@@ -19322,12 +19355,12 @@
       <c r="Q35" s="1">
         <v>0.442424242424242</v>
       </c>
-      <c r="R35" s="12">
+      <c r="R35" s="9">
         <v>0.48848484848484802</v>
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="1">
@@ -19375,12 +19408,12 @@
       <c r="Q36" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R36" s="12">
+      <c r="R36" s="9">
         <v>0.62060606060606005</v>
       </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="1">
@@ -19428,12 +19461,12 @@
       <c r="Q37" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R37" s="12">
+      <c r="R37" s="9">
         <v>0.69010101010100999</v>
       </c>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="1">
@@ -19481,12 +19514,12 @@
       <c r="Q38" s="1">
         <v>0.381818181818181</v>
       </c>
-      <c r="R38" s="12">
+      <c r="R38" s="9">
         <v>0.49414141414141399</v>
       </c>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="1">
@@ -19534,7 +19567,7 @@
       <c r="Q39" s="1">
         <v>0.39393939393939298</v>
       </c>
-      <c r="R39" s="12">
+      <c r="R39" s="9">
         <v>0.44484848484848399</v>
       </c>
     </row>
@@ -19571,60 +19604,60 @@
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="G45" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="H45" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I45" s="11" t="s">
+      <c r="I45" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="J45" s="11" t="s">
+      <c r="J45" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="K45" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L45" s="11" t="s">
+      <c r="L45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M45" s="11" t="s">
+      <c r="M45" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N45" s="11" t="s">
+      <c r="N45" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O45" s="11" t="s">
+      <c r="O45" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="P45" s="11" t="s">
+      <c r="P45" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q45" s="11" t="s">
+      <c r="Q45" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R45" s="11" t="s">
+      <c r="R45" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="1">
@@ -19672,13 +19705,13 @@
       <c r="Q46" s="1">
         <v>0.30909090909090903</v>
       </c>
-      <c r="R46" s="12">
+      <c r="R46" s="9">
         <v>0.39474747474747401</v>
       </c>
       <c r="S46" s="1"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C47" s="1">
@@ -19726,13 +19759,13 @@
       <c r="Q47" s="1">
         <v>0.37575757575757501</v>
       </c>
-      <c r="R47" s="12">
+      <c r="R47" s="9">
         <v>0.45494949494949399</v>
       </c>
       <c r="S47" s="1"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C48" s="1">
@@ -19780,13 +19813,13 @@
       <c r="Q48" s="1">
         <v>0.218181818181818</v>
       </c>
-      <c r="R48" s="12">
+      <c r="R48" s="9">
         <v>0.409696969696969</v>
       </c>
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C49" s="1">
@@ -19834,13 +19867,13 @@
       <c r="Q49" s="1">
         <v>0.218181818181818</v>
       </c>
-      <c r="R49" s="12">
+      <c r="R49" s="9">
         <v>0.47515151515151499</v>
       </c>
       <c r="S49" s="1"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="1">
@@ -19888,13 +19921,13 @@
       <c r="Q50" s="1">
         <v>0.26060606060606001</v>
       </c>
-      <c r="R50" s="12">
+      <c r="R50" s="9">
         <v>0.48080808080808002</v>
       </c>
       <c r="S50" s="1"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="1">
@@ -19942,13 +19975,13 @@
       <c r="Q51" s="1">
         <v>0.43030303030303002</v>
       </c>
-      <c r="R51" s="12">
+      <c r="R51" s="9">
         <v>0.39919191919191899</v>
       </c>
       <c r="S51" s="1"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="1">
@@ -19996,7 +20029,7 @@
       <c r="Q52" s="1">
         <v>0.47878787878787799</v>
       </c>
-      <c r="R52" s="12">
+      <c r="R52" s="9">
         <v>0.38585858585858501</v>
       </c>
       <c r="S52" s="1"/>
@@ -20034,60 +20067,60 @@
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D58" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E58" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G58" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H58" s="11" t="s">
+      <c r="H58" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I58" s="11" t="s">
+      <c r="I58" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="J58" s="11" t="s">
+      <c r="J58" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K58" s="11" t="s">
+      <c r="K58" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L58" s="11" t="s">
+      <c r="L58" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M58" s="11" t="s">
+      <c r="M58" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N58" s="11" t="s">
+      <c r="N58" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O58" s="11" t="s">
+      <c r="O58" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="P58" s="11" t="s">
+      <c r="P58" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q58" s="11" t="s">
+      <c r="Q58" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R58" s="11" t="s">
+      <c r="R58" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="1">
@@ -20135,12 +20168,12 @@
       <c r="Q59" s="1">
         <v>0.49090909090909002</v>
       </c>
-      <c r="R59" s="12">
+      <c r="R59" s="9">
         <v>0.46303030303030301</v>
       </c>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C60" s="1">
@@ -20188,12 +20221,12 @@
       <c r="Q60" s="1">
         <v>0.527272727272727</v>
       </c>
-      <c r="R60" s="12">
+      <c r="R60" s="9">
         <v>0.51434343434343399</v>
       </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C61" s="1">
@@ -20241,12 +20274,12 @@
       <c r="Q61" s="1">
         <v>0.38787878787878699</v>
       </c>
-      <c r="R61" s="12">
+      <c r="R61" s="9">
         <v>0.44525252525252501</v>
       </c>
     </row>
     <row r="62" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C62" s="1">
@@ -20294,12 +20327,12 @@
       <c r="Q62" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R62" s="12">
+      <c r="R62" s="9">
         <v>0.61414141414141399</v>
       </c>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="1">
@@ -20347,12 +20380,12 @@
       <c r="Q63" s="1">
         <v>0.50303030303030305</v>
       </c>
-      <c r="R63" s="12">
+      <c r="R63" s="9">
         <v>0.67555555555555502</v>
       </c>
     </row>
     <row r="64" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="1">
@@ -20400,12 +20433,12 @@
       <c r="Q64" s="1">
         <v>0.37575757575757501</v>
       </c>
-      <c r="R64" s="12">
+      <c r="R64" s="9">
         <v>0.472727272727272</v>
       </c>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="1">
@@ -20453,7 +20486,7 @@
       <c r="Q65" s="1">
         <v>0.39393939393939298</v>
       </c>
-      <c r="R65" s="12">
+      <c r="R65" s="9">
         <v>0.43151515151515102</v>
       </c>
     </row>
@@ -20490,60 +20523,60 @@
       </c>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="D71" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="E71" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F71" s="11" t="s">
+      <c r="F71" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G71" s="11" t="s">
+      <c r="G71" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H71" s="11" t="s">
+      <c r="H71" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I71" s="11" t="s">
+      <c r="I71" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="J71" s="11" t="s">
+      <c r="J71" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="K71" s="11" t="s">
+      <c r="K71" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="L71" s="11" t="s">
+      <c r="L71" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M71" s="11" t="s">
+      <c r="M71" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="N71" s="11" t="s">
+      <c r="N71" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="O71" s="11" t="s">
+      <c r="O71" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="P71" s="11" t="s">
+      <c r="P71" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q71" s="11" t="s">
+      <c r="Q71" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="R71" s="11" t="s">
+      <c r="R71" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C72" s="1">
@@ -20591,12 +20624,12 @@
       <c r="Q72" s="1">
         <v>0.31515151515151502</v>
       </c>
-      <c r="R72" s="12">
+      <c r="R72" s="9">
         <v>0.38787878787878699</v>
       </c>
     </row>
     <row r="73" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C73" s="1">
@@ -20644,12 +20677,12 @@
       <c r="Q73" s="1">
         <v>0.30909090909090903</v>
       </c>
-      <c r="R73" s="12">
+      <c r="R73" s="9">
         <v>0.41131313131313102</v>
       </c>
     </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C74" s="1">
@@ -20697,12 +20730,12 @@
       <c r="Q74" s="1">
         <v>0.206060606060606</v>
       </c>
-      <c r="R74" s="12">
+      <c r="R74" s="9">
         <v>0.419797979797979</v>
       </c>
     </row>
     <row r="75" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C75" s="1">
@@ -20750,12 +20783,12 @@
       <c r="Q75" s="1">
         <v>0.206060606060606</v>
       </c>
-      <c r="R75" s="12">
+      <c r="R75" s="9">
         <v>0.48363636363636298</v>
       </c>
     </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C76" s="1">
@@ -20803,12 +20836,12 @@
       <c r="Q76" s="1">
         <v>0.26060606060606001</v>
       </c>
-      <c r="R76" s="12">
+      <c r="R76" s="9">
         <v>0.48323232323232301</v>
       </c>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C77" s="1">
@@ -20856,12 +20889,12 @@
       <c r="Q77" s="1">
         <v>0.43636363636363601</v>
       </c>
-      <c r="R77" s="12">
+      <c r="R77" s="9">
         <v>0.39151515151515098</v>
       </c>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C78" s="1">
@@ -20909,7 +20942,7 @@
       <c r="Q78" s="1">
         <v>0.47878787878787799</v>
       </c>
-      <c r="R78" s="12">
+      <c r="R78" s="9">
         <v>0.383030303030302</v>
       </c>
     </row>
@@ -20922,8 +20955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AI32" sqref="AI32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20932,12 +20965,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="13">
+      <c r="B1" s="10">
         <v>100200</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
@@ -20960,173 +20993,173 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <v>0.51742424242424201</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="11">
         <v>0.50227272727272698</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="11">
         <v>0.49204545454545401</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="11">
         <v>0.42159090909090902</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="11">
         <v>0.39280303030302999</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="11">
         <v>0.391666666666666</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>0.52803030303030296</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>0.53219696969696895</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="11">
         <v>0.495075757575757</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="11">
         <v>0.43409090909090903</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="11">
         <v>0.41477272727272702</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="11">
         <v>0.44015151515151502</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <v>0.52196969696969697</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <v>0.49696969696969601</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <v>0.52386363636363598</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="11">
         <v>0.423863636363636</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <v>0.40681818181818102</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="11">
         <v>0.414015151515151</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>0.55378787878787805</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>0.58333333333333304</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <v>0.57348484848484804</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <v>0.460984848484848</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="11">
         <v>0.47499999999999898</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="11">
         <v>0.472727272727272</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>0.58825757575757498</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>0.62386363636363595</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="11">
         <v>0.63712121212121198</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="11">
         <v>0.46136363636363598</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="11">
         <v>0.47992424242424198</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="11">
         <v>0.47613636363636302</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>0.51780303030302999</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>0.48977272727272703</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="11">
         <v>0.49545454545454498</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <v>0.444318181818181</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="11">
         <v>0.43522727272727202</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="11">
         <v>0.44545454545454499</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="11">
         <v>0.52045454545454495</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <v>0.47992424242424198</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <v>0.483333333333333</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <v>0.44280303030302998</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="11">
         <v>0.423863636363636</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="11">
         <v>0.43143939393939301</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="B13" s="10">
         <v>250500</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C14" t="s">
@@ -21149,163 +21182,163 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="11">
         <v>0.55434343434343403</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="11">
         <v>0.42707070707070699</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="11">
         <v>0.46303030303030301</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="11">
         <v>0.414545454545454</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="11">
         <v>0.39474747474747401</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="11">
         <v>0.38787878787878699</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="11">
         <v>0.53696969696969699</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="11">
         <v>0.49050505050505</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="11">
         <v>0.51434343434343399</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="11">
         <v>0.41616161616161601</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="11">
         <v>0.45494949494949399</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="11">
         <v>0.41131313131313102</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="11">
         <v>0.54101010101010105</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="11">
         <v>0.48848484848484802</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="11">
         <v>0.44525252525252501</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="11">
         <v>0.43030303030303002</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="11">
         <v>0.409696969696969</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="11">
         <v>0.419797979797979</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="11">
         <v>0.61212121212121196</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="11">
         <v>0.62060606060606005</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="11">
         <v>0.61414141414141399</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="11">
         <v>0.44282828282828202</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="11">
         <v>0.47515151515151499</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="11">
         <v>0.48363636363636298</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="11">
         <v>0.61777777777777698</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="11">
         <v>0.69010101010100999</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="11">
         <v>0.67555555555555502</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="11">
         <v>0.46343434343434298</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="11">
         <v>0.48080808080808002</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="11">
         <v>0.48323232323232301</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="11">
         <v>0.56525252525252501</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="11">
         <v>0.49414141414141399</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="11">
         <v>0.472727272727272</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="11">
         <v>0.42303030303030298</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="11">
         <v>0.39919191919191899</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="11">
         <v>0.39151515151515098</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="11">
         <v>0.55515151515151495</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="11">
         <v>0.44484848484848399</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="11">
         <v>0.43151515151515102</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <v>0.41696969696969599</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="11">
         <v>0.38585858585858501</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="11">
         <v>0.383030303030302</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add results and make program to count points
</commit_message>
<xml_diff>
--- a/data/sumup/results.xlsx
+++ b/data/sumup/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="16065" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="klasyczne podejscie " sheetId="1" r:id="rId1"/>
@@ -17,17 +17,6 @@
     <sheet name="n fold 250 500" sheetId="4" r:id="rId3"/>
     <sheet name="n fold chart" sheetId="3" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'klasyczne podejscie '!$F$6:$F$16</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'klasyczne podejscie '!$K$55</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'klasyczne podejscie '!$K$56:$K$66</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'klasyczne podejscie '!$L$55</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'klasyczne podejscie '!$L$56:$L$66</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'klasyczne podejscie '!$M$55</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'klasyczne podejscie '!$M$56:$M$66</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'klasyczne podejscie '!$N$55</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'klasyczne podejscie '!$N$56:$N$66</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -454,10 +443,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3939,7 +3928,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4336,7 +4324,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4433,7 +4420,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4508,7 +4494,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4620,7 +4605,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5084,7 +5068,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5180,7 +5163,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5248,7 +5230,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5345,7 +5326,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5686,7 +5666,6 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5783,7 +5762,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5851,7 +5829,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5943,7 +5920,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6308,7 +6284,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6410,7 +6385,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6458,7 +6432,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10152,7 +10125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+    <sheetView topLeftCell="D7" workbookViewId="0">
       <selection activeCell="AH85" sqref="AH85"/>
     </sheetView>
   </sheetViews>
@@ -10181,18 +10154,18 @@
       <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>8</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13">
         <v>16</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
     </row>
     <row r="5" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -10598,18 +10571,18 @@
       <c r="F21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>8</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14">
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13">
         <v>16</v>
       </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
     </row>
     <row r="22" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F22" s="3" t="s">
@@ -10998,18 +10971,18 @@
       <c r="F37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>8</v>
       </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14">
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13">
         <v>16</v>
       </c>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
     </row>
     <row r="38" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F38" s="3" t="s">
@@ -11425,18 +11398,18 @@
       <c r="F54" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G54" s="13">
+      <c r="G54" s="14">
         <v>8</v>
       </c>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13">
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14">
         <v>16</v>
       </c>
-      <c r="L54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="13"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
     </row>
     <row r="55" spans="5:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F55" s="3" t="s">
@@ -11803,22 +11776,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="E6:E12"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="K37:N37"/>
     <mergeCell ref="E63:E66"/>
     <mergeCell ref="E39:E45"/>
     <mergeCell ref="E46:E49"/>
     <mergeCell ref="G54:J54"/>
     <mergeCell ref="K54:N54"/>
     <mergeCell ref="E56:E62"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="E6:E12"/>
+    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11830,7 +11803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AQ77"/>
   <sheetViews>
-    <sheetView topLeftCell="L25" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="AQ5" sqref="AQ5:AQ77"/>
     </sheetView>
   </sheetViews>
@@ -20955,7 +20928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AI32" sqref="AI32"/>
     </sheetView>
   </sheetViews>

</xml_diff>